<commit_message>
update PNP transistors in BOM
</commit_message>
<xml_diff>
--- a/bom/base_convert_A.xlsx
+++ b/bom/base_convert_A.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Dropbox\KiCAD\projects\base_convert\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0E6BF011-03D7-496A-BFBB-0458480BC07F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DBA8EB-9DBD-4013-A507-77A799C907D5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_convert_A" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="217">
   <si>
     <t>Description</t>
   </si>
@@ -262,9 +262,6 @@
     <t>SI2323DDS-T1-GE3</t>
   </si>
   <si>
-    <t>TRANS PNP 40V 0.2A SOT23</t>
-  </si>
-  <si>
     <t>Q_PNP_BEC</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>Nexperia USA Inc.</t>
   </si>
   <si>
-    <t>PMBT3906,235</t>
-  </si>
-  <si>
     <t>RES SMD 102K OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -631,9 +625,6 @@
     <t>94500A212</t>
   </si>
   <si>
-    <t>1727-1885-1-ND </t>
-  </si>
-  <si>
     <t>Build Cost</t>
   </si>
   <si>
@@ -659,15 +650,36 @@
   </si>
   <si>
     <t>Payment Processing Fee 4% + $0.3</t>
+  </si>
+  <si>
+    <t>PDTA123ET,215</t>
+  </si>
+  <si>
+    <t>1727-1691-1-ND </t>
+  </si>
+  <si>
+    <t>TRANS PREBIAS PNP 250MW TO236AB</t>
+  </si>
+  <si>
+    <t>LED Display Lens</t>
+  </si>
+  <si>
+    <t>Hammond Manufacturing</t>
+  </si>
+  <si>
+    <t>1593SIR10</t>
+  </si>
+  <si>
+    <t>HM889-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1170,11 +1182,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="44"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1367,27 +1379,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P34" totalsRowCount="1" dataDxfId="6" dataCellStyle="Currency">
-  <autoFilter ref="A1:P33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P35" totalsRowCount="1" dataDxfId="6" dataCellStyle="Currency">
+  <autoFilter ref="A1:P34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="Description"/>
-    <tableColumn id="2" name="Part"/>
-    <tableColumn id="3" name="References"/>
-    <tableColumn id="4" name="Value"/>
-    <tableColumn id="5" name="Footprint"/>
-    <tableColumn id="6" name="Quantity Per PCB"/>
-    <tableColumn id="7" name="Datasheet"/>
-    <tableColumn id="8" name="Manufacture"/>
-    <tableColumn id="9" name="Package"/>
-    <tableColumn id="10" name="Mfg Part Number"/>
-    <tableColumn id="11" name="Supplier"/>
-    <tableColumn id="12" name="Supplier Part Number" dataCellStyle="Hyperlink" totalsRowCellStyle="Hyperlink"/>
-    <tableColumn id="13" name="Purchased Qty"/>
-    <tableColumn id="14" name="Price" dataDxfId="5" totalsRowDxfId="2" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
-    <tableColumn id="15" name="Cost Per Unit" dataDxfId="4" totalsRowDxfId="1" dataCellStyle="Currency" totalsRowCellStyle="Currency">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Description"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="References"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Footprint"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Quantity Per PCB"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Datasheet"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Manufacture"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Package"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Mfg Part Number"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Supplier"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Supplier Part Number" dataCellStyle="Hyperlink" totalsRowCellStyle="Hyperlink"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Purchased Qty"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Price" dataDxfId="5" totalsRowDxfId="2" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cost Per Unit" dataDxfId="4" totalsRowDxfId="1" dataCellStyle="Currency" totalsRowCellStyle="Currency">
       <calculatedColumnFormula>N2/M2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Cost Per PCB" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="0" dataCellStyle="Currency" totalsRowCellStyle="Currency">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Cost Per PCB" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="0" dataCellStyle="Currency" totalsRowCellStyle="Currency">
       <calculatedColumnFormula>O2*F2</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table1[Cost Per PCB])</totalsRowFormula>
     </tableColumn>
@@ -1692,11 +1704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,22 +1762,22 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" t="s">
         <v>145</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>146</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>147</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>148</v>
-      </c>
-      <c r="O1" t="s">
-        <v>149</v>
-      </c>
-      <c r="P1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1800,10 +1812,10 @@
         <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M2">
         <v>6</v>
@@ -1853,10 +1865,10 @@
         <v>24</v>
       </c>
       <c r="K3" t="s">
+        <v>149</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="M3">
         <v>500</v>
@@ -1902,13 +1914,13 @@
         <v>805</v>
       </c>
       <c r="J4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M4">
         <v>100</v>
@@ -1957,10 +1969,10 @@
         <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M5">
         <v>500</v>
@@ -1985,10 +1997,10 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
@@ -2009,10 +2021,10 @@
         <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M6">
         <v>160</v>
@@ -2061,10 +2073,10 @@
         <v>41</v>
       </c>
       <c r="K7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M7">
         <v>35</v>
@@ -2084,7 +2096,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
@@ -2096,28 +2108,28 @@
         <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" t="s">
         <v>141</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>142</v>
       </c>
-      <c r="I8" t="s">
-        <v>143</v>
-      </c>
-      <c r="J8" t="s">
-        <v>144</v>
-      </c>
       <c r="K8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -2166,10 +2178,10 @@
         <v>58</v>
       </c>
       <c r="K9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="M9">
         <v>10</v>
@@ -2188,7 +2200,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2197,13 +2209,13 @@
         <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M10">
         <v>10</v>
@@ -2222,7 +2234,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -2231,13 +2243,13 @@
         <v>56</v>
       </c>
       <c r="J11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="M11">
         <v>100</v>
@@ -2286,10 +2298,10 @@
         <v>66</v>
       </c>
       <c r="K12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M12">
         <v>1000</v>
@@ -2338,10 +2350,10 @@
         <v>73</v>
       </c>
       <c r="K13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M13">
         <f>100+100</f>
@@ -2392,10 +2404,10 @@
         <v>79</v>
       </c>
       <c r="K14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="M14">
         <v>10</v>
@@ -2414,16 +2426,16 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" t="s">
         <v>80</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>81</v>
       </c>
-      <c r="C15" t="s">
-        <v>82</v>
-      </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
         <v>70</v>
@@ -2432,74 +2444,74 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" t="s">
         <v>83</v>
-      </c>
-      <c r="H15" t="s">
-        <v>84</v>
       </c>
       <c r="I15" t="s">
         <v>70</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>210</v>
       </c>
       <c r="K15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="M15">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="N15" s="3">
-        <v>5.18</v>
+        <v>3.36</v>
       </c>
       <c r="O15" s="3">
         <f t="shared" si="0"/>
-        <v>5.1799999999999999E-2</v>
+        <v>0.16799999999999998</v>
       </c>
       <c r="P15" s="3">
         <f t="shared" si="1"/>
-        <v>0.72519999999999996</v>
+        <v>2.3519999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
         <v>86</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>87</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>88</v>
-      </c>
-      <c r="D16" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" t="s">
-        <v>90</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I16">
         <v>603</v>
       </c>
       <c r="J16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M16">
         <v>2500</v>
@@ -2518,40 +2530,40 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" t="s">
         <v>94</v>
       </c>
-      <c r="B17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" t="s">
-        <v>96</v>
-      </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I17">
         <v>603</v>
       </c>
       <c r="J17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="M17">
         <v>408</v>
@@ -2570,40 +2582,40 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D18">
         <v>150</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F18">
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I18">
         <v>1206</v>
       </c>
       <c r="J18" t="s">
+        <v>170</v>
+      </c>
+      <c r="K18" t="s">
+        <v>149</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="K18" t="s">
-        <v>151</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="M18">
         <v>30</v>
@@ -2622,40 +2634,40 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" t="s">
         <v>98</v>
-      </c>
-      <c r="C19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" t="s">
-        <v>100</v>
       </c>
       <c r="F19">
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I19">
         <v>1206</v>
       </c>
       <c r="J19" t="s">
+        <v>173</v>
+      </c>
+      <c r="K19" t="s">
+        <v>149</v>
+      </c>
+      <c r="L19" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="K19" t="s">
-        <v>151</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="M19">
         <v>50</v>
@@ -2674,40 +2686,40 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" t="s">
         <v>105</v>
-      </c>
-      <c r="B20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" t="s">
-        <v>137</v>
-      </c>
-      <c r="D20" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" t="s">
-        <v>107</v>
       </c>
       <c r="F20">
         <v>17</v>
       </c>
       <c r="G20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" t="s">
+        <v>107</v>
+      </c>
+      <c r="I20" t="s">
         <v>108</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>109</v>
       </c>
-      <c r="I20" t="s">
-        <v>110</v>
-      </c>
-      <c r="J20" t="s">
-        <v>111</v>
-      </c>
       <c r="K20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M20">
         <f>18+100</f>
@@ -2728,40 +2740,40 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" t="s">
         <v>112</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>113</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>114</v>
-      </c>
-      <c r="D21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" t="s">
-        <v>116</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" t="s">
         <v>117</v>
       </c>
-      <c r="H21" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" t="s">
-        <v>118</v>
-      </c>
-      <c r="J21" t="s">
-        <v>119</v>
-      </c>
       <c r="K21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M21">
         <f>5+4</f>
@@ -2782,40 +2794,40 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" t="s">
         <v>120</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>121</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>122</v>
-      </c>
-      <c r="D22" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" t="s">
-        <v>124</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H22" t="s">
+        <v>124</v>
+      </c>
+      <c r="I22" t="s">
         <v>125</v>
       </c>
-      <c r="H22" t="s">
-        <v>126</v>
-      </c>
-      <c r="I22" t="s">
-        <v>127</v>
-      </c>
       <c r="J22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M22">
         <v>50</v>
@@ -2834,40 +2846,40 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="s">
         <v>128</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" t="s">
         <v>129</v>
-      </c>
-      <c r="C23" t="s">
-        <v>130</v>
-      </c>
-      <c r="D23" t="s">
-        <v>129</v>
-      </c>
-      <c r="E23" t="s">
-        <v>131</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H23" t="s">
+        <v>131</v>
+      </c>
+      <c r="I23" t="s">
         <v>132</v>
       </c>
-      <c r="H23" t="s">
-        <v>133</v>
-      </c>
-      <c r="I23" t="s">
-        <v>134</v>
-      </c>
       <c r="J23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M23">
         <f>2+5</f>
@@ -2888,22 +2900,22 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F24">
         <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M24">
         <v>100</v>
@@ -2922,7 +2934,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F25">
         <v>8</v>
@@ -2934,10 +2946,10 @@
         <v>971100151</v>
       </c>
       <c r="K25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M25">
         <v>50</v>
@@ -2946,17 +2958,17 @@
         <v>19.8</v>
       </c>
       <c r="O25" s="3">
-        <f>N25/M25</f>
+        <f t="shared" ref="O25:O34" si="4">N25/M25</f>
         <v>0.39600000000000002</v>
       </c>
       <c r="P25" s="3">
-        <f>O25*F25</f>
+        <f t="shared" ref="P25:P34" si="5">O25*F25</f>
         <v>3.1680000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -2968,10 +2980,10 @@
         <v>970180151</v>
       </c>
       <c r="K26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M26">
         <v>50</v>
@@ -2980,377 +2992,412 @@
         <v>22.88</v>
       </c>
       <c r="O26" s="3">
-        <f>N26/M26</f>
+        <f t="shared" si="4"/>
         <v>0.45760000000000001</v>
       </c>
       <c r="P26" s="3">
-        <f>O26*F26</f>
+        <f t="shared" si="5"/>
         <v>3.6608000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>193</v>
+        <v>214</v>
+      </c>
+      <c r="J27" t="s">
+        <v>215</v>
       </c>
       <c r="K27" t="s">
-        <v>193</v>
-      </c>
-      <c r="L27" s="2"/>
+        <v>149</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="M27">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N27" s="3">
-        <f>5+(35.94/5)</f>
-        <v>12.187999999999999</v>
+        <v>2.58</v>
       </c>
       <c r="O27" s="3">
         <f>N27/M27</f>
-        <v>1.2187999999999999</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="P27" s="3">
         <f>O27*F27</f>
-        <v>1.2187999999999999</v>
+        <v>1.032</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28">
         <v>10</v>
       </c>
       <c r="N28" s="3">
-        <f>2+(35.94/5)</f>
-        <v>9.1879999999999988</v>
+        <f>5+(35.94/5)</f>
+        <v>12.187999999999999</v>
       </c>
       <c r="O28" s="3">
-        <f>N28/M28</f>
-        <v>0.91879999999999984</v>
+        <f t="shared" si="4"/>
+        <v>1.2187999999999999</v>
       </c>
       <c r="P28" s="3">
-        <f>O28*F28</f>
-        <v>0.91879999999999984</v>
+        <f t="shared" si="5"/>
+        <v>1.2187999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29">
         <v>10</v>
       </c>
       <c r="N29" s="3">
+        <f>2+(35.94/5)</f>
+        <v>9.1879999999999988</v>
+      </c>
+      <c r="O29" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91879999999999984</v>
+      </c>
+      <c r="P29" s="3">
+        <f t="shared" si="5"/>
+        <v>0.91879999999999984</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>190</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>191</v>
+      </c>
+      <c r="K30" t="s">
+        <v>191</v>
+      </c>
+      <c r="L30" s="2"/>
+      <c r="M30">
+        <v>10</v>
+      </c>
+      <c r="N30" s="3">
         <f>5+(35.94/5)</f>
         <v>12.187999999999999</v>
       </c>
-      <c r="O29" s="3">
-        <f>N29/M29</f>
+      <c r="O30" s="3">
+        <f t="shared" si="4"/>
         <v>1.2187999999999999</v>
       </c>
-      <c r="P29" s="3">
-        <f>O29*F29</f>
+      <c r="P30" s="3">
+        <f t="shared" si="5"/>
         <v>1.2187999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>196</v>
-      </c>
-      <c r="F30">
-        <v>16</v>
-      </c>
-      <c r="H30" t="s">
-        <v>194</v>
-      </c>
-      <c r="J30" t="s">
-        <v>202</v>
-      </c>
-      <c r="K30" t="s">
-        <v>194</v>
-      </c>
-      <c r="L30" s="2"/>
-      <c r="M30">
-        <v>100</v>
-      </c>
-      <c r="N30" s="3">
-        <v>11.66</v>
-      </c>
-      <c r="O30" s="3">
-        <f>N30/M30</f>
-        <v>0.1166</v>
-      </c>
-      <c r="P30" s="3">
-        <f>O30*F30</f>
-        <v>1.8655999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="H31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J31" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31">
         <v>100</v>
       </c>
       <c r="N31" s="3">
-        <v>8.58</v>
+        <v>11.66</v>
       </c>
       <c r="O31" s="3">
-        <f>N31/M31</f>
-        <v>8.5800000000000001E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.1166</v>
       </c>
       <c r="P31" s="3">
-        <f>O31*F31</f>
-        <v>0.1716</v>
+        <f t="shared" si="5"/>
+        <v>1.8655999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F32">
         <v>2</v>
       </c>
       <c r="H32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J32" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N32" s="3">
-        <v>8.76</v>
+        <v>8.58</v>
       </c>
       <c r="O32" s="3">
-        <f>N32/M32</f>
-        <v>0.17519999999999999</v>
+        <f t="shared" si="4"/>
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="P32" s="3">
-        <f>O32*F32</f>
-        <v>0.35039999999999999</v>
+        <f t="shared" si="5"/>
+        <v>0.1716</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F33">
         <v>2</v>
       </c>
       <c r="H33" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J33" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K33" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33">
+        <v>50</v>
+      </c>
+      <c r="N33" s="3">
+        <v>8.76</v>
+      </c>
+      <c r="O33" s="3">
+        <f t="shared" si="4"/>
+        <v>0.17519999999999999</v>
+      </c>
+      <c r="P33" s="3">
+        <f t="shared" si="5"/>
+        <v>0.35039999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>198</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>192</v>
+      </c>
+      <c r="J34" t="s">
+        <v>199</v>
+      </c>
+      <c r="K34" t="s">
+        <v>192</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="M34">
         <v>100</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N34" s="3">
         <v>2.27</v>
       </c>
-      <c r="O33" s="3">
-        <f>N33/M33</f>
+      <c r="O34" s="3">
+        <f t="shared" si="4"/>
         <v>2.2700000000000001E-2</v>
       </c>
-      <c r="P33" s="3">
-        <f>O33*F33</f>
+      <c r="P34" s="3">
+        <f t="shared" si="5"/>
         <v>4.5400000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L34" s="2"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L35" s="2"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3">
         <f>SUM(Table1[Cost Per PCB])</f>
-        <v>41.333424586146322</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+        <v>43.992224586146335</v>
+      </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="3">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="3">
         <f>SUM(Table1[Cost Per PCB])</f>
-        <v>41.333424586146322</v>
-      </c>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>205</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="4">
+        <v>43.992224586146335</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="4">
         <v>2.5</v>
-      </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="11">
-        <f>C36*C37</f>
-        <v>103.3335614653658</v>
       </c>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B39" s="7"/>
-      <c r="C39" s="3">
-        <v>3.68</v>
+      <c r="C39" s="11">
+        <f>C37*C38</f>
+        <v>109.98056146536584</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B40" s="7"/>
-      <c r="C40" s="11">
-        <f>C38+C39</f>
-        <v>107.01356146536581</v>
+      <c r="C40" s="3">
+        <v>3.68</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B41" s="7"/>
-      <c r="C41" s="12">
-        <f>C40*5%</f>
-        <v>5.3506780732682913</v>
+      <c r="C41" s="11">
+        <f>C39+C40</f>
+        <v>113.66056146536584</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="12">
-        <f>(C40*4%)+0.3</f>
-        <v>4.5805424586146319</v>
-      </c>
-      <c r="D42" s="3">
-        <v>0.3</v>
-      </c>
+        <f>C41*5%</f>
+        <v>5.683028073268293</v>
+      </c>
+      <c r="D42" s="4"/>
       <c r="F42" s="8"/>
-      <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="11">
-        <f>C40-C41-C42</f>
-        <v>97.082340933482882</v>
-      </c>
-      <c r="D43" s="4"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="12">
+        <f>(C41*4%)+0.3</f>
+        <v>4.8464224586146338</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B44" s="10"/>
+        <v>206</v>
+      </c>
+      <c r="B44" s="9"/>
       <c r="C44" s="11">
-        <f>C43-C36</f>
-        <v>55.748916347336561</v>
+        <f>C41-C42-C43</f>
+        <v>103.13111093348292</v>
       </c>
       <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="11">
+        <f>C44-C37</f>
+        <v>59.13888634733658</v>
+      </c>
+      <c r="D45" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" display="https://www.digikey.com/product-detail/en/mpd-memory-protection-devices/BC4AAW/BC4AAW-ND/66733"/>
-    <hyperlink ref="L3" r:id="rId2" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL21B104KOANNNC/1276-2448-1-ND/3890534"/>
-    <hyperlink ref="L4" r:id="rId3" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL21A106MQFNNNE/1276-1298-1-ND/3889384"/>
-    <hyperlink ref="L5" r:id="rId4" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL21B105KOFNNNG/1276-6471-1-ND/5958099"/>
-    <hyperlink ref="L6" r:id="rId5" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080RS75000/732-4984-1-ND/4489916"/>
-    <hyperlink ref="L7" r:id="rId6" display="https://www.digikey.com/product-detail/en/lite-on-inc/LTD-2601WC/160-2244-ND/3199017"/>
-    <hyperlink ref="L9" r:id="rId7" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/S2B-PH-K-S(LF)(SN)/455-1719-ND/926626"/>
-    <hyperlink ref="L10" r:id="rId8" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/PHR-2/455-1165-ND/608607"/>
-    <hyperlink ref="L11" r:id="rId9" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/SPH-002T-P0.5L/455-2148-1-ND/1634657"/>
-    <hyperlink ref="L12" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RC1206JR-070RL/311-0.0ERCT-ND/732131"/>
-    <hyperlink ref="L13" r:id="rId11" display="https://www.digikey.com/product-detail/en/taiwan-semiconductor-corporation/MMBT3904L-RFG/MMBT3904LRFGCT-ND/7357839"/>
-    <hyperlink ref="L14" r:id="rId12" display="https://www.digikey.com/product-detail/en/vishay-siliconix/SI2323DDS-T1-GE3/SI2323DDS-T1-GE3CT-ND/4142086"/>
-    <hyperlink ref="L16" r:id="rId13" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MCR03ERTF1023/RHM102KCFCT-ND/4083896"/>
-    <hyperlink ref="L17" r:id="rId14" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MCR03ERTF2552/RHM25.5KCFCT-ND/4084087"/>
-    <hyperlink ref="L18" r:id="rId15" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MNR34J5ABJ151/MNR34151CT-ND/657596"/>
-    <hyperlink ref="L19" r:id="rId16" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MNR34J5ABJ562/MNR34562CT-ND/657638"/>
-    <hyperlink ref="L20" r:id="rId17" display="https://www.digikey.com/product-detail/en/c-k/PTS645SK13SMTR92LFS/CKN10817CT-ND/7056128"/>
-    <hyperlink ref="L21" r:id="rId18" display="https://www.digikey.com/product-detail/en/c-k/SS-24E06-TG-5-(P)/CKN10394-ND/2747191"/>
-    <hyperlink ref="L22" r:id="rId19" display="https://www.digikey.com/product-detail/en/microchip-technology/MIC5317-3.3YM5-TR/MIC5317-3.3YM5-CT-ND/7671939"/>
-    <hyperlink ref="L23" r:id="rId20" display="https://www.digikey.com/product-detail/en/texas-instruments/MSP430FR2033IPMR/296-48617-1-ND/8567661"/>
-    <hyperlink ref="L24" r:id="rId21" display="https://www.digikey.com/product-detail/en/bivar-inc/VLP-450-R/492-1347-ND/586475"/>
-    <hyperlink ref="L25" r:id="rId22" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/971100151/732-10397-ND/6174616"/>
-    <hyperlink ref="L26" r:id="rId23" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/970180151/732-10586-ND/6174806"/>
-    <hyperlink ref="L15" r:id="rId24" display="https://www.digikey.com/product-detail/en/nexperia-usa-inc/PMBT3906,235/1727-1885-1-ND/5015560"/>
+    <hyperlink ref="L2" r:id="rId1" display="https://www.digikey.com/product-detail/en/mpd-memory-protection-devices/BC4AAW/BC4AAW-ND/66733" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL21B104KOANNNC/1276-2448-1-ND/3890534" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL21A106MQFNNNE/1276-1298-1-ND/3889384" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="L5" r:id="rId4" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL21B105KOFNNNG/1276-6471-1-ND/5958099" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="L6" r:id="rId5" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080RS75000/732-4984-1-ND/4489916" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="L7" r:id="rId6" display="https://www.digikey.com/product-detail/en/lite-on-inc/LTD-2601WC/160-2244-ND/3199017" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="L9" r:id="rId7" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/S2B-PH-K-S(LF)(SN)/455-1719-ND/926626" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="L10" r:id="rId8" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/PHR-2/455-1165-ND/608607" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="L11" r:id="rId9" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/SPH-002T-P0.5L/455-2148-1-ND/1634657" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="L12" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RC1206JR-070RL/311-0.0ERCT-ND/732131" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="L13" r:id="rId11" display="https://www.digikey.com/product-detail/en/taiwan-semiconductor-corporation/MMBT3904L-RFG/MMBT3904LRFGCT-ND/7357839" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="L14" r:id="rId12" display="https://www.digikey.com/product-detail/en/vishay-siliconix/SI2323DDS-T1-GE3/SI2323DDS-T1-GE3CT-ND/4142086" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="L16" r:id="rId13" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MCR03ERTF1023/RHM102KCFCT-ND/4083896" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="L17" r:id="rId14" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MCR03ERTF2552/RHM25.5KCFCT-ND/4084087" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="L18" r:id="rId15" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MNR34J5ABJ151/MNR34151CT-ND/657596" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="L19" r:id="rId16" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MNR34J5ABJ562/MNR34562CT-ND/657638" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="L20" r:id="rId17" display="https://www.digikey.com/product-detail/en/c-k/PTS645SK13SMTR92LFS/CKN10817CT-ND/7056128" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="L21" r:id="rId18" display="https://www.digikey.com/product-detail/en/c-k/SS-24E06-TG-5-(P)/CKN10394-ND/2747191" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L22" r:id="rId19" display="https://www.digikey.com/product-detail/en/microchip-technology/MIC5317-3.3YM5-TR/MIC5317-3.3YM5-CT-ND/7671939" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L23" r:id="rId20" display="https://www.digikey.com/product-detail/en/texas-instruments/MSP430FR2033IPMR/296-48617-1-ND/8567661" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L24" r:id="rId21" display="https://www.digikey.com/product-detail/en/bivar-inc/VLP-450-R/492-1347-ND/586475" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="L25" r:id="rId22" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/971100151/732-10397-ND/6174616" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L26" r:id="rId23" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/970180151/732-10586-ND/6174806" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L15" r:id="rId24" display="https://www.digikey.com/product-detail/en/nexperia-usa-inc/PDTA123ET,215/1727-1691-1-ND/4581217" xr:uid="{449FE790-90DE-4B15-B29A-C80A494FCD4B}"/>
+    <hyperlink ref="L27" r:id="rId25" display="https://www.digikey.com/product-detail/en/hammond-manufacturing/1593SIR10/HM889-ND/409899" xr:uid="{3C4860AB-AA1C-4407-A88E-79B91083F147}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId25"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId26"/>
   <tableParts count="1">
-    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update BOM with PNP and 10k RN
</commit_message>
<xml_diff>
--- a/bom/base_convert_A.xlsx
+++ b/bom/base_convert_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Dropbox\KiCAD\projects\base_convert\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DBA8EB-9DBD-4013-A507-77A799C907D5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026A0AB0-46F8-4EB6-BA8D-291D7C74FEA4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="221">
   <si>
     <t>Description</t>
   </si>
@@ -322,9 +322,6 @@
     <t>http://rohmfs.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor_network/mnr_g.pdf</t>
   </si>
   <si>
-    <t>RN1 RN3 RN4 RN5 RN6 RN9 RN10</t>
-  </si>
-  <si>
     <t>4.7k</t>
   </si>
   <si>
@@ -671,6 +668,21 @@
   </si>
   <si>
     <t>HM889-ND</t>
+  </si>
+  <si>
+    <t>RES ARRAY 4 RES 10K OHM 2012</t>
+  </si>
+  <si>
+    <t>RN1 RN4 RN5 RN6</t>
+  </si>
+  <si>
+    <t>RN3 RN9 RN10</t>
+  </si>
+  <si>
+    <t>YC324-JK-0710KL</t>
+  </si>
+  <si>
+    <t>YC324J-10KCT-ND</t>
   </si>
 </sst>
 </file>
@@ -1379,8 +1391,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P35" totalsRowCount="1" dataDxfId="6" dataCellStyle="Currency">
-  <autoFilter ref="A1:P34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P36" totalsRowCount="1" dataDxfId="6" dataCellStyle="Currency">
+  <autoFilter ref="A1:P35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Description"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part"/>
@@ -1705,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,22 +1774,22 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" t="s">
         <v>143</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>144</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>145</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>146</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>147</v>
-      </c>
-      <c r="P1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1812,10 +1824,10 @@
         <v>11</v>
       </c>
       <c r="K2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="M2">
         <v>6</v>
@@ -1865,10 +1877,10 @@
         <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M3">
         <v>500</v>
@@ -1877,11 +1889,11 @@
         <v>4.43</v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" ref="O3:O23" si="0">N3/M3</f>
+        <f t="shared" ref="O3:O24" si="0">N3/M3</f>
         <v>8.8599999999999998E-3</v>
       </c>
       <c r="P3" s="3">
-        <f t="shared" ref="P3:P23" si="1">O3*F3</f>
+        <f t="shared" ref="P3:P24" si="1">O3*F3</f>
         <v>8.8599999999999998E-3</v>
       </c>
     </row>
@@ -1914,13 +1926,13 @@
         <v>805</v>
       </c>
       <c r="J4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K4" t="s">
+        <v>148</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="K4" t="s">
-        <v>149</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="M4">
         <v>100</v>
@@ -1969,10 +1981,10 @@
         <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M5">
         <v>500</v>
@@ -1997,10 +2009,10 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" t="s">
         <v>133</v>
-      </c>
-      <c r="D6" t="s">
-        <v>134</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
@@ -2021,10 +2033,10 @@
         <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M6">
         <v>160</v>
@@ -2073,10 +2085,10 @@
         <v>41</v>
       </c>
       <c r="K7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M7">
         <v>35</v>
@@ -2096,7 +2108,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
@@ -2108,28 +2120,28 @@
         <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" t="s">
         <v>139</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>140</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>141</v>
       </c>
-      <c r="J8" t="s">
-        <v>142</v>
-      </c>
       <c r="K8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -2178,10 +2190,10 @@
         <v>58</v>
       </c>
       <c r="K9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M9">
         <v>10</v>
@@ -2200,7 +2212,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2209,13 +2221,13 @@
         <v>56</v>
       </c>
       <c r="J10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K10" t="s">
+        <v>148</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="K10" t="s">
-        <v>149</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="M10">
         <v>10</v>
@@ -2234,7 +2246,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -2243,13 +2255,13 @@
         <v>56</v>
       </c>
       <c r="J11" t="s">
+        <v>162</v>
+      </c>
+      <c r="K11" t="s">
+        <v>148</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="K11" t="s">
-        <v>149</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="M11">
         <v>100</v>
@@ -2298,10 +2310,10 @@
         <v>66</v>
       </c>
       <c r="K12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M12">
         <v>1000</v>
@@ -2350,10 +2362,10 @@
         <v>73</v>
       </c>
       <c r="K13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M13">
         <f>100+100</f>
@@ -2404,10 +2416,10 @@
         <v>79</v>
       </c>
       <c r="K14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M14">
         <v>10</v>
@@ -2426,7 +2438,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B15" t="s">
         <v>80</v>
@@ -2453,13 +2465,13 @@
         <v>70</v>
       </c>
       <c r="J15" t="s">
+        <v>209</v>
+      </c>
+      <c r="K15" t="s">
+        <v>148</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="K15" t="s">
-        <v>149</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="M15">
         <v>20</v>
@@ -2508,10 +2520,10 @@
         <v>91</v>
       </c>
       <c r="K16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M16">
         <v>2500</v>
@@ -2560,10 +2572,10 @@
         <v>95</v>
       </c>
       <c r="K17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M17">
         <v>408</v>
@@ -2582,7 +2594,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B18" t="s">
         <v>96</v>
@@ -2609,13 +2621,13 @@
         <v>1206</v>
       </c>
       <c r="J18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M18">
         <v>30</v>
@@ -2634,25 +2646,25 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
         <v>96</v>
       </c>
       <c r="C19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" t="s">
         <v>100</v>
-      </c>
-      <c r="D19" t="s">
-        <v>101</v>
       </c>
       <c r="E19" t="s">
         <v>98</v>
       </c>
       <c r="F19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H19" t="s">
         <v>90</v>
@@ -2661,13 +2673,13 @@
         <v>1206</v>
       </c>
       <c r="J19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M19">
         <v>50</v>
@@ -2681,294 +2693,297 @@
       </c>
       <c r="P19" s="3">
         <f t="shared" si="1"/>
-        <v>0.91139999999999988</v>
+        <v>0.39059999999999995</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" t="s">
+        <v>217</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" t="s">
+        <v>219</v>
+      </c>
+      <c r="K20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="M20">
+        <v>50</v>
+      </c>
+      <c r="N20" s="3">
+        <v>7.97</v>
+      </c>
+      <c r="O20" s="3">
+        <f>N20/M20</f>
+        <v>0.15939999999999999</v>
+      </c>
+      <c r="P20" s="3">
+        <f>O20*F20</f>
+        <v>0.63759999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" t="s">
         <v>103</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" t="s">
         <v>104</v>
       </c>
-      <c r="C20" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" t="s">
-        <v>136</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F21">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
         <v>105</v>
       </c>
-      <c r="F20">
-        <v>17</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H21" t="s">
         <v>106</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I21" t="s">
         <v>107</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J21" t="s">
         <v>108</v>
       </c>
-      <c r="J20" t="s">
-        <v>109</v>
-      </c>
-      <c r="K20" t="s">
-        <v>149</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="M20">
+      <c r="K21" t="s">
+        <v>148</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="M21">
         <f>18+100</f>
         <v>118</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N21" s="3">
         <f>6.34+27.66</f>
         <v>34</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O21" s="3">
         <f t="shared" si="0"/>
         <v>0.28813559322033899</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P21" s="3">
         <f t="shared" si="1"/>
         <v>4.898305084745763</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" t="s">
         <v>110</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C22" t="s">
         <v>111</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D22" t="s">
         <v>112</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E22" t="s">
         <v>113</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>114</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="H22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" t="s">
         <v>115</v>
       </c>
-      <c r="H21" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="J22" t="s">
         <v>116</v>
       </c>
-      <c r="J21" t="s">
-        <v>117</v>
-      </c>
-      <c r="K21" t="s">
-        <v>149</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="M21">
+      <c r="K22" t="s">
+        <v>148</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="M22">
         <f>5+4</f>
         <v>9</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N22" s="3">
         <f>4.2+3.36</f>
         <v>7.5600000000000005</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O22" s="3">
         <f t="shared" si="0"/>
         <v>0.84000000000000008</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P22" s="3">
         <f t="shared" si="1"/>
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" t="s">
         <v>118</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C23" t="s">
         <v>119</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D23" t="s">
         <v>120</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E23" t="s">
         <v>121</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
         <v>122</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="H23" t="s">
         <v>123</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I23" t="s">
         <v>124</v>
       </c>
-      <c r="I22" t="s">
-        <v>125</v>
-      </c>
-      <c r="J22" t="s">
-        <v>121</v>
-      </c>
-      <c r="K22" t="s">
-        <v>149</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="M22">
+      <c r="J23" t="s">
+        <v>120</v>
+      </c>
+      <c r="K23" t="s">
+        <v>148</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="M23">
         <v>50</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N23" s="3">
         <v>6.7</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O23" s="3">
         <f t="shared" si="0"/>
         <v>0.13400000000000001</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P23" s="3">
         <f t="shared" si="1"/>
         <v>0.13400000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" t="s">
         <v>126</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C24" t="s">
         <v>127</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" t="s">
         <v>128</v>
       </c>
-      <c r="D23" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
         <v>129</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H24" t="s">
         <v>130</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I24" t="s">
         <v>131</v>
       </c>
-      <c r="I23" t="s">
-        <v>132</v>
-      </c>
-      <c r="J23" t="s">
-        <v>127</v>
-      </c>
-      <c r="K23" t="s">
-        <v>149</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="M23">
+      <c r="J24" t="s">
+        <v>126</v>
+      </c>
+      <c r="K24" t="s">
+        <v>148</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M24">
         <f>2+5</f>
         <v>7</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N24" s="3">
         <f>5.2+13</f>
         <v>18.2</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O24" s="3">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="P23" s="3">
+      <c r="P24" s="3">
         <f t="shared" si="1"/>
         <v>2.6</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>181</v>
-      </c>
-      <c r="F24">
-        <v>16</v>
-      </c>
-      <c r="H24" t="s">
-        <v>182</v>
-      </c>
-      <c r="J24" t="s">
-        <v>183</v>
-      </c>
-      <c r="K24" t="s">
-        <v>149</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="M24">
-        <v>100</v>
-      </c>
-      <c r="N24" s="3">
-        <v>29.23</v>
-      </c>
-      <c r="O24" s="3">
-        <f t="shared" ref="O24" si="2">N24/M24</f>
-        <v>0.2923</v>
-      </c>
-      <c r="P24" s="3">
-        <f t="shared" ref="P24" si="3">O24*F24</f>
-        <v>4.6768000000000001</v>
-      </c>
-    </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F25">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H25" t="s">
-        <v>38</v>
-      </c>
-      <c r="J25">
-        <v>971100151</v>
+        <v>181</v>
+      </c>
+      <c r="J25" t="s">
+        <v>182</v>
       </c>
       <c r="K25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="M25">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N25" s="3">
-        <v>19.8</v>
+        <v>29.23</v>
       </c>
       <c r="O25" s="3">
-        <f t="shared" ref="O25:O34" si="4">N25/M25</f>
-        <v>0.39600000000000002</v>
+        <f t="shared" ref="O25" si="2">N25/M25</f>
+        <v>0.2923</v>
       </c>
       <c r="P25" s="3">
-        <f t="shared" ref="P25:P34" si="5">O25*F25</f>
-        <v>3.1680000000000001</v>
+        <f t="shared" ref="P25" si="3">O25*F25</f>
+        <v>4.6768000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -2977,183 +2992,185 @@
         <v>38</v>
       </c>
       <c r="J26">
-        <v>970180151</v>
+        <v>971100151</v>
       </c>
       <c r="K26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M26">
         <v>50</v>
       </c>
       <c r="N26" s="3">
+        <v>19.8</v>
+      </c>
+      <c r="O26" s="3">
+        <f t="shared" ref="O26:O35" si="4">N26/M26</f>
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="P26" s="3">
+        <f t="shared" ref="P26:P35" si="5">O26*F26</f>
+        <v>3.1680000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>185</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+      <c r="H27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J27">
+        <v>970180151</v>
+      </c>
+      <c r="K27" t="s">
+        <v>148</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="M27">
+        <v>50</v>
+      </c>
+      <c r="N27" s="3">
         <v>22.88</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O27" s="3">
         <f t="shared" si="4"/>
         <v>0.45760000000000001</v>
       </c>
-      <c r="P26" s="3">
+      <c r="P27" s="3">
         <f t="shared" si="5"/>
         <v>3.6608000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>213</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="H27" t="s">
-        <v>214</v>
-      </c>
-      <c r="J27" t="s">
-        <v>215</v>
-      </c>
-      <c r="K27" t="s">
-        <v>149</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="M27">
-        <v>5</v>
-      </c>
-      <c r="N27" s="3">
-        <v>2.58</v>
-      </c>
-      <c r="O27" s="3">
-        <f>N27/M27</f>
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="P27" s="3">
-        <f>O27*F27</f>
-        <v>1.032</v>
-      </c>
-    </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>191</v>
+        <v>213</v>
+      </c>
+      <c r="J28" t="s">
+        <v>214</v>
       </c>
       <c r="K28" t="s">
-        <v>191</v>
-      </c>
-      <c r="L28" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="M28">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N28" s="3">
-        <f>5+(35.94/5)</f>
-        <v>12.187999999999999</v>
+        <v>2.58</v>
       </c>
       <c r="O28" s="3">
-        <f t="shared" si="4"/>
-        <v>1.2187999999999999</v>
+        <f>N28/M28</f>
+        <v>0.51600000000000001</v>
       </c>
       <c r="P28" s="3">
-        <f t="shared" si="5"/>
-        <v>1.2187999999999999</v>
+        <f>O28*F28</f>
+        <v>1.032</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29">
         <v>10</v>
       </c>
       <c r="N29" s="3">
-        <f>2+(35.94/5)</f>
-        <v>9.1879999999999988</v>
+        <f>5+(35.94/5)</f>
+        <v>12.187999999999999</v>
       </c>
       <c r="O29" s="3">
         <f t="shared" si="4"/>
-        <v>0.91879999999999984</v>
+        <v>1.2187999999999999</v>
       </c>
       <c r="P29" s="3">
         <f t="shared" si="5"/>
-        <v>0.91879999999999984</v>
+        <v>1.2187999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30">
         <v>10</v>
       </c>
       <c r="N30" s="3">
+        <f>2+(35.94/5)</f>
+        <v>9.1879999999999988</v>
+      </c>
+      <c r="O30" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91879999999999984</v>
+      </c>
+      <c r="P30" s="3">
+        <f t="shared" si="5"/>
+        <v>0.91879999999999984</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>190</v>
+      </c>
+      <c r="K31" t="s">
+        <v>190</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31">
+        <v>10</v>
+      </c>
+      <c r="N31" s="3">
         <f>5+(35.94/5)</f>
         <v>12.187999999999999</v>
       </c>
-      <c r="O30" s="3">
+      <c r="O31" s="3">
         <f t="shared" si="4"/>
         <v>1.2187999999999999</v>
       </c>
-      <c r="P30" s="3">
+      <c r="P31" s="3">
         <f t="shared" si="5"/>
         <v>1.2187999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>194</v>
-      </c>
-      <c r="F31">
-        <v>16</v>
-      </c>
-      <c r="H31" t="s">
-        <v>192</v>
-      </c>
-      <c r="J31" t="s">
-        <v>200</v>
-      </c>
-      <c r="K31" t="s">
-        <v>192</v>
-      </c>
-      <c r="L31" s="2"/>
-      <c r="M31">
-        <v>100</v>
-      </c>
-      <c r="N31" s="3">
-        <v>11.66</v>
-      </c>
-      <c r="O31" s="3">
-        <f t="shared" si="4"/>
-        <v>0.1166</v>
-      </c>
-      <c r="P31" s="3">
-        <f t="shared" si="5"/>
-        <v>1.8655999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3161,210 +3178,242 @@
         <v>193</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="H32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J32" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32">
         <v>100</v>
       </c>
       <c r="N32" s="3">
-        <v>8.58</v>
+        <v>11.66</v>
       </c>
       <c r="O32" s="3">
         <f t="shared" si="4"/>
-        <v>8.5800000000000001E-2</v>
+        <v>0.1166</v>
       </c>
       <c r="P32" s="3">
         <f t="shared" si="5"/>
-        <v>0.1716</v>
+        <v>1.8655999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F33">
         <v>2</v>
       </c>
       <c r="H33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J33" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N33" s="3">
-        <v>8.76</v>
+        <v>8.58</v>
       </c>
       <c r="O33" s="3">
         <f t="shared" si="4"/>
-        <v>0.17519999999999999</v>
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="P33" s="3">
         <f t="shared" si="5"/>
-        <v>0.35039999999999999</v>
+        <v>0.1716</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F34">
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J34" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="N34" s="3">
-        <v>2.27</v>
+        <v>8.76</v>
       </c>
       <c r="O34" s="3">
         <f t="shared" si="4"/>
-        <v>2.2700000000000001E-2</v>
+        <v>0.17519999999999999</v>
       </c>
       <c r="P34" s="3">
         <f t="shared" si="5"/>
+        <v>0.35039999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>197</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>191</v>
+      </c>
+      <c r="J35" t="s">
+        <v>198</v>
+      </c>
+      <c r="K35" t="s">
+        <v>191</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="M35">
+        <v>100</v>
+      </c>
+      <c r="N35" s="3">
+        <v>2.27</v>
+      </c>
+      <c r="O35" s="3">
+        <f t="shared" si="4"/>
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="P35" s="3">
+        <f t="shared" si="5"/>
         <v>4.5400000000000003E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L35" s="2"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L36" s="2"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3">
         <f>SUM(Table1[Cost Per PCB])</f>
-        <v>43.992224586146335</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+        <v>44.109024586146333</v>
+      </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="3">
+        <f>SUM(Table1[Cost Per PCB])</f>
+        <v>44.109024586146333</v>
+      </c>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>201</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="3">
-        <f>SUM(Table1[Cost Per PCB])</f>
-        <v>43.992224586146335</v>
-      </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>202</v>
-      </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="4">
+      <c r="B39" s="6"/>
+      <c r="C39" s="4">
         <v>2.5</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="11">
-        <f>C37*C38</f>
-        <v>109.98056146536584</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B40" s="7"/>
-      <c r="C40" s="3">
-        <v>3.68</v>
+      <c r="C40" s="11">
+        <f>C38*C39</f>
+        <v>110.27256146536584</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B41" s="7"/>
-      <c r="C41" s="11">
-        <f>C39+C40</f>
-        <v>113.66056146536584</v>
+      <c r="C41" s="3">
+        <v>3.68</v>
       </c>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B42" s="7"/>
-      <c r="C42" s="12">
-        <f>C41*5%</f>
-        <v>5.683028073268293</v>
+      <c r="C42" s="11">
+        <f>C40+C41</f>
+        <v>113.95256146536585</v>
       </c>
       <c r="D42" s="4"/>
-      <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="12">
-        <f>(C41*4%)+0.3</f>
-        <v>4.8464224586146338</v>
-      </c>
-      <c r="D43" s="3">
-        <v>0.3</v>
-      </c>
+        <f>C42*5%</f>
+        <v>5.6976280732682927</v>
+      </c>
+      <c r="D43" s="4"/>
       <c r="F43" s="8"/>
-      <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="11">
-        <f>C41-C42-C43</f>
-        <v>103.13111093348292</v>
-      </c>
-      <c r="D44" s="4"/>
+        <v>208</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="12">
+        <f>(C42*4%)+0.3</f>
+        <v>4.858102458614634</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="B45" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="B45" s="9"/>
       <c r="C45" s="11">
-        <f>C44-C37</f>
-        <v>59.13888634733658</v>
+        <f>C42-C43-C44</f>
+        <v>103.39683093348292</v>
       </c>
       <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="11">
+        <f>C45-C38</f>
+        <v>59.287806347336584</v>
+      </c>
+      <c r="D46" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3384,20 +3433,21 @@
     <hyperlink ref="L17" r:id="rId14" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MCR03ERTF2552/RHM25.5KCFCT-ND/4084087" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="L18" r:id="rId15" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MNR34J5ABJ151/MNR34151CT-ND/657596" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="L19" r:id="rId16" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/MNR34J5ABJ562/MNR34562CT-ND/657638" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="L20" r:id="rId17" display="https://www.digikey.com/product-detail/en/c-k/PTS645SK13SMTR92LFS/CKN10817CT-ND/7056128" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="L21" r:id="rId18" display="https://www.digikey.com/product-detail/en/c-k/SS-24E06-TG-5-(P)/CKN10394-ND/2747191" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="L22" r:id="rId19" display="https://www.digikey.com/product-detail/en/microchip-technology/MIC5317-3.3YM5-TR/MIC5317-3.3YM5-CT-ND/7671939" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="L23" r:id="rId20" display="https://www.digikey.com/product-detail/en/texas-instruments/MSP430FR2033IPMR/296-48617-1-ND/8567661" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="L24" r:id="rId21" display="https://www.digikey.com/product-detail/en/bivar-inc/VLP-450-R/492-1347-ND/586475" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="L25" r:id="rId22" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/971100151/732-10397-ND/6174616" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="L26" r:id="rId23" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/970180151/732-10586-ND/6174806" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L21" r:id="rId17" display="https://www.digikey.com/product-detail/en/c-k/PTS645SK13SMTR92LFS/CKN10817CT-ND/7056128" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="L22" r:id="rId18" display="https://www.digikey.com/product-detail/en/c-k/SS-24E06-TG-5-(P)/CKN10394-ND/2747191" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L23" r:id="rId19" display="https://www.digikey.com/product-detail/en/microchip-technology/MIC5317-3.3YM5-TR/MIC5317-3.3YM5-CT-ND/7671939" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L24" r:id="rId20" display="https://www.digikey.com/product-detail/en/texas-instruments/MSP430FR2033IPMR/296-48617-1-ND/8567661" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L25" r:id="rId21" display="https://www.digikey.com/product-detail/en/bivar-inc/VLP-450-R/492-1347-ND/586475" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="L26" r:id="rId22" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/971100151/732-10397-ND/6174616" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L27" r:id="rId23" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/970180151/732-10586-ND/6174806" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="L15" r:id="rId24" display="https://www.digikey.com/product-detail/en/nexperia-usa-inc/PDTA123ET,215/1727-1691-1-ND/4581217" xr:uid="{449FE790-90DE-4B15-B29A-C80A494FCD4B}"/>
-    <hyperlink ref="L27" r:id="rId25" display="https://www.digikey.com/product-detail/en/hammond-manufacturing/1593SIR10/HM889-ND/409899" xr:uid="{3C4860AB-AA1C-4407-A88E-79B91083F147}"/>
+    <hyperlink ref="L28" r:id="rId25" display="https://www.digikey.com/product-detail/en/hammond-manufacturing/1593SIR10/HM889-ND/409899" xr:uid="{3C4860AB-AA1C-4407-A88E-79B91083F147}"/>
+    <hyperlink ref="L20" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/YC324-JK-0710KL/YC324J-10KCT-ND/1005865" xr:uid="{D154DE7E-C457-4D1B-8205-C7B1CA7E071F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId26"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId27"/>
   <tableParts count="1">
-    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>